<commit_message>
created revision B of hardware enables native usb support with usb capable stm32 uploading firmware is possible over USB-DFU
</commit_message>
<xml_diff>
--- a/Electronics/Knobber/Project Outputs for Knobber/Release_B00/No Variant/[No Variations]_VariantRevision_Knobber_BOM.xlsx
+++ b/Electronics/Knobber/Project Outputs for Knobber/Release_B00/No Variant/[No Variations]_VariantRevision_Knobber_BOM.xlsx
@@ -70,7 +70,7 @@
     <t>23.02.2025</t>
   </si>
   <si>
-    <t>14:03</t>
+    <t>17:04</t>
   </si>
   <si>
     <t>&lt;Parameter GBS_2.0_Parameter not found&gt;</t>
@@ -1221,7 +1221,7 @@
       </c>
       <c r="C9" s="44">
         <f ca="1">NOW()</f>
-        <v>45711.58607451389</v>
+        <v>45711.71123253472</v>
       </c>
       <c r="D9"/>
       <c r="E9" s="7"/>

</xml_diff>